<commit_message>
checking in update with blueSource_Users page (excelSheet)
</commit_message>
<xml_diff>
--- a/src/main/resources/excelsheets/blueSource_Users.xlsx
+++ b/src/main/resources/excelsheets/blueSource_Users.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>company.admin</t>
   </si>
@@ -45,6 +45,18 @@
   </si>
   <si>
     <t>User Name</t>
+  </si>
+  <si>
+    <t>Account Name</t>
+  </si>
+  <si>
+    <t>Account1</t>
+  </si>
+  <si>
+    <t>Account2</t>
+  </si>
+  <si>
+    <t>Account3</t>
   </si>
 </sst>
 </file>
@@ -396,56 +408,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes to accounts_search (update)
</commit_message>
<xml_diff>
--- a/src/main/resources/excelsheets/blueSource_Users.xlsx
+++ b/src/main/resources/excelsheets/blueSource_Users.xlsx
@@ -53,10 +53,10 @@
     <t>Account1</t>
   </si>
   <si>
-    <t>Account2</t>
-  </si>
-  <si>
-    <t>Account3</t>
+    <t>department1 m1e1</t>
+  </si>
+  <si>
+    <t>department1 m1e2</t>
   </si>
 </sst>
 </file>
@@ -411,14 +411,14 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -451,7 +451,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -462,7 +462,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -473,7 +473,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes made to accounts_test_search
</commit_message>
<xml_diff>
--- a/src/main/resources/excelsheets/blueSource_Users.xlsx
+++ b/src/main/resources/excelsheets/blueSource_Users.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>company.admin</t>
   </si>
@@ -45,18 +45,6 @@
   </si>
   <si>
     <t>User Name</t>
-  </si>
-  <si>
-    <t>Account Name</t>
-  </si>
-  <si>
-    <t>Account1</t>
-  </si>
-  <si>
-    <t>department1 m1e1</t>
-  </si>
-  <si>
-    <t>department1 m1e2</t>
   </si>
 </sst>
 </file>
@@ -408,7 +396,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
@@ -421,59 +409,44 @@
     <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>